<commit_message>
with rdps and file transfers
</commit_message>
<xml_diff>
--- a/documentation/Integrations Endpoints .xlsx
+++ b/documentation/Integrations Endpoints .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC07723\Documents\tsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2C879BF-DD67-49CD-B4FD-ABC1F8525493}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68388294-72D2-43B5-BF38-C25D00E0D4B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0FC83C2E-5F6F-4EE0-ADF4-D969216C56BF}"/>
+    <workbookView xWindow="690" yWindow="345" windowWidth="18420" windowHeight="12960" activeTab="1" xr2:uid="{0FC83C2E-5F6F-4EE0-ADF4-D969216C56BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Creditflow" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="249">
   <si>
     <t>Procedure Name</t>
   </si>
@@ -805,6 +805,21 @@
   </si>
   <si>
     <t>BigIP PROD</t>
+  </si>
+  <si>
+    <t>RDP</t>
+  </si>
+  <si>
+    <t>d99, d100, t66, t67, p21, p22, p26, u27</t>
+  </si>
+  <si>
+    <t>File transfer</t>
+  </si>
+  <si>
+    <t>137-139, 445</t>
+  </si>
+  <si>
+    <t>udp &amp; tcp</t>
   </si>
 </sst>
 </file>
@@ -2527,11 +2542,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0544C5E6-7A51-4759-B20A-CF2156EBEB66}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,7 +2554,7 @@
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="89.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3132,6 +3147,37 @@
         <v>80</v>
       </c>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>244</v>
+      </c>
+      <c r="B48" t="s">
+        <v>238</v>
+      </c>
+      <c r="C48" t="s">
+        <v>245</v>
+      </c>
+      <c r="D48">
+        <v>3389</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" t="s">
+        <v>238</v>
+      </c>
+      <c r="C49" t="s">
+        <v>245</v>
+      </c>
+      <c r="D49" t="s">
+        <v>247</v>
+      </c>
+      <c r="E49" t="s">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>